<commit_message>
changes to payroll along with gitignores
</commit_message>
<xml_diff>
--- a/Server/Required_files/HDL_BO_Hierarchy_All_Objects_Charlie.xlsx
+++ b/Server/Required_files/HDL_BO_Hierarchy_All_Objects_Charlie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GIT\Project_Charlie_Main\Server\Required_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\GitHub\Charlie_Backup\Project_Charlie_Main\Server\Required_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8040F4-4CC3-4EC2-8D9E-35438D113814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFFC374-6C86-4703-AB9F-96E6C6385196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$140</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1561,11 +1561,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J140" sqref="J140"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1636,7 +1637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1928,7 +1929,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2041,7 +2042,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -2122,7 +2123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2148,7 +2149,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -2174,7 +2175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -2288,7 +2289,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -2393,7 +2394,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -2498,7 +2499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -2574,7 +2575,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -2606,7 +2607,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -2670,7 +2671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -2702,7 +2703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -2728,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -2786,7 +2787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>109</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -2867,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>113</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>115</v>
       </c>
@@ -2922,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>117</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -2977,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>121</v>
       </c>
@@ -3006,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>125</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -3110,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>131</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>133</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>135</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>137</v>
       </c>
@@ -3214,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>139</v>
       </c>
@@ -3243,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>141</v>
       </c>
@@ -3269,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>143</v>
       </c>
@@ -3295,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>145</v>
       </c>
@@ -3454,7 +3455,7 @@
         <v>150</v>
       </c>
       <c r="G64" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="H64" t="s">
         <v>161</v>
@@ -3486,7 +3487,7 @@
         <v>150</v>
       </c>
       <c r="G65" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="H65" t="s">
         <v>161</v>
@@ -3512,7 +3513,7 @@
         <v>150</v>
       </c>
       <c r="G66" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="H66" t="s">
         <v>161</v>
@@ -3538,7 +3539,7 @@
         <v>150</v>
       </c>
       <c r="G67" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="H67" t="s">
         <v>161</v>
@@ -3608,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>175</v>
       </c>
@@ -3640,7 +3641,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>180</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -3692,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -3724,7 +3725,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>188</v>
       </c>
@@ -3782,7 +3783,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -3814,7 +3815,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>198</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>200</v>
       </c>
@@ -3866,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>202</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>206</v>
       </c>
@@ -3944,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>208</v>
       </c>
@@ -3976,7 +3977,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>212</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>215</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>219</v>
       </c>
@@ -4078,7 +4079,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>222</v>
       </c>
@@ -4110,7 +4111,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>226</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>230</v>
       </c>
@@ -4302,7 +4303,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>246</v>
       </c>
@@ -4334,7 +4335,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>250</v>
       </c>
@@ -4360,7 +4361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>252</v>
       </c>
@@ -4386,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>254</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>256</v>
       </c>
@@ -4438,7 +4439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>258</v>
       </c>
@@ -4470,7 +4471,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>262</v>
       </c>
@@ -4502,7 +4503,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>267</v>
       </c>
@@ -4528,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>269</v>
       </c>
@@ -4554,7 +4555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>271</v>
       </c>
@@ -4580,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>273</v>
       </c>
@@ -4606,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>275</v>
       </c>
@@ -4632,7 +4633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>277</v>
       </c>
@@ -4664,7 +4665,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>282</v>
       </c>
@@ -4690,7 +4691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>284</v>
       </c>
@@ -4722,7 +4723,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>288</v>
       </c>
@@ -4748,7 +4749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>290</v>
       </c>
@@ -4774,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>292</v>
       </c>
@@ -4803,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>294</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>296</v>
       </c>
@@ -4861,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>298</v>
       </c>
@@ -4887,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>300</v>
       </c>
@@ -4913,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>302</v>
       </c>
@@ -4939,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>304</v>
       </c>
@@ -4965,7 +4966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>306</v>
       </c>
@@ -4991,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>307</v>
       </c>
@@ -5017,7 +5018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>309</v>
       </c>
@@ -5043,7 +5044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>311</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>313</v>
       </c>
@@ -5101,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>315</v>
       </c>
@@ -5127,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>317</v>
       </c>
@@ -5159,7 +5160,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>321</v>
       </c>
@@ -5185,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>323</v>
       </c>
@@ -5211,7 +5212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>325</v>
       </c>
@@ -5237,7 +5238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>327</v>
       </c>
@@ -5269,7 +5270,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>331</v>
       </c>
@@ -5295,7 +5296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>333</v>
       </c>
@@ -5321,7 +5322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>335</v>
       </c>
@@ -5347,7 +5348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>367</v>
       </c>
@@ -5367,7 +5368,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>364</v>
       </c>
@@ -5387,7 +5388,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>337</v>
       </c>
@@ -5419,7 +5420,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>341</v>
       </c>
@@ -5445,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>343</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>345</v>
       </c>
@@ -5535,7 +5536,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>371</v>
       </c>
@@ -5555,7 +5556,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>375</v>
       </c>
@@ -5578,7 +5579,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>378</v>
       </c>
@@ -5605,19 +5606,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P137" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P140" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Payroll"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:M1 A3:M36 A2:L2 A109:L119 A38 C38:L38 A39:L39 A40:L59 A60:L60 A61:L61 A62:L63 A64 C64:L64 A65:L65 A66:L67 A68:L68 A69:L69 A70:L70 A71:L71 A72:L72 A73:L73 A74:L74 A75 C75:F75 A76:L76 A77:L77 A78:L81 A82:G82 I82:L82 A83:L83 A84:L84 A85:L85 A86:G86 I86:L86 A87:L87 A88:L88 A89:L89 A90:L90 A92:H92 A93:L93 A94:L94 A95:L97 A98:L98 A99:L99 A100:L100 A101:L104 A105:G105 I105:L105 A106:L106 A107:L107 A137:L137 A120:L120 A108:L108 A121:L121 A122:L122 A123:L123 A124:L124 A125:L126 A127:G127 I127:L127 A128:L128 A129:L130 A133:L133 A134:L134 A135:L135 A136:G136 I136:L136 A37:L37 H75:L75 J92:L92" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:M1 A3:M36 A2:L2 A109:L119 A38 C38:L38 A39:L39 A40:L59 A60:L60 A61:L61 A62:L63 A64 C64:F64 A65:F65 A66:F67 A68:L68 A69:L69 A70:L70 A71:L71 A72:L72 A73:L73 A74:L74 A75 C75:F75 A76:L76 A77:L77 A78:L81 A82:G82 I82:L82 A83:L83 A84:L84 A85:L85 A86:G86 I86:L86 A87:L87 A88:L88 A89:L89 A90:L90 A92:H92 A93:L93 A94:L94 A95:L97 A98:L98 A99:L99 A100:L100 A101:L104 A105:G105 I105:L105 A106:L106 A107:L107 A137:L137 A120:L120 A108:L108 A121:L121 A122:L122 A123:L123 A124:L124 A125:L126 A127:G127 I127:L127 A128:L128 A129:L130 A133:L133 A134:L134 A135:L135 A136:G136 I136:L136 A37:L37 H75:L75 J92:L92 H64:L64 H65:L65 H66:L67" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5783,26 +5793,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3604BF4-0FFF-4404-B039-B7C228E8F270}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DD9110C-7E4A-451C-B6FE-5459C4D27920}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="eda7b593-5b33-4455-9f72-a492af41ea7a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5826,9 +5825,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DD9110C-7E4A-451C-B6FE-5459C4D27920}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3604BF4-0FFF-4404-B039-B7C228E8F270}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="eda7b593-5b33-4455-9f72-a492af41ea7a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>